<commit_message>
Agreement contests appear to all be working correctly, with nearly identical results for rmdm.
</commit_message>
<xml_diff>
--- a/mdm_z/atherosclerosis_review.xlsx
+++ b/mdm_z/atherosclerosis_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\CodeProjects\ACE\mdm_z\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A7A2F1-1109-4734-88A6-9C29BBB07728}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52B987F-1BCA-4665-9B81-D9028466413B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
+    <workbookView xWindow="5460" yWindow="2655" windowWidth="18960" windowHeight="11835" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chol Null" sheetId="2" r:id="rId1"/>
@@ -10144,7 +10144,7 @@
   <dimension ref="A1:AK49"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10256,7 +10256,7 @@
     </row>
     <row r="3" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>0.183950949515405</v>
+        <v>0.119467592853033</v>
       </c>
       <c r="B3" s="16">
         <v>0.119216677992623</v>
@@ -10322,7 +10322,7 @@
     </row>
     <row r="4" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
-        <v>0.27440793954739701</v>
+        <v>0.16567496718522901</v>
       </c>
       <c r="B4" s="16">
         <v>0.165311568236927</v>
@@ -10385,7 +10385,7 @@
     </row>
     <row r="5" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
-        <v>0.38436459197423101</v>
+        <v>0.17759148857781601</v>
       </c>
       <c r="B5" s="16">
         <v>0.20433837829325699</v>
@@ -10450,7 +10450,7 @@
     </row>
     <row r="6" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <v>0.40203950808969302</v>
+        <v>0.234556114439678</v>
       </c>
       <c r="B6" s="16">
         <v>0.23210822869911099</v>
@@ -10513,7 +10513,7 @@
     </row>
     <row r="7" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
-        <v>0.44662961215296099</v>
+        <v>0.27813693178833598</v>
       </c>
       <c r="B7" s="16">
         <v>0.27521663080706799</v>
@@ -10578,7 +10578,7 @@
     </row>
     <row r="8" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
-        <v>0.43928376831671601</v>
+        <v>0.29060090781743703</v>
       </c>
       <c r="B8" s="16">
         <v>0.28959587906393203</v>
@@ -10641,7 +10641,7 @@
     </row>
     <row r="9" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
-        <v>0.56936456603711305</v>
+        <v>0.35372837090937498</v>
       </c>
       <c r="B9" s="16">
         <v>0.35724301949486198</v>
@@ -10705,7 +10705,7 @@
     </row>
     <row r="10" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
-        <v>1.0857575240092801</v>
+        <v>0.69484648624400702</v>
       </c>
       <c r="B10" s="16">
         <v>0.68915117283806204</v>
@@ -10770,7 +10770,7 @@
     </row>
     <row r="11" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
-        <v>2.0143047983429199</v>
+        <v>1.13419239366617</v>
       </c>
       <c r="B11" s="16">
         <v>0.93512532884303801</v>
@@ -13612,7 +13612,7 @@
   <dimension ref="A1:AK44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -13739,7 +13739,7 @@
     </row>
     <row r="3" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
-        <v>0.19558591730595501</v>
+        <v>0.13441159242109799</v>
       </c>
       <c r="B3" s="16">
         <v>0.134149932094661</v>
@@ -13802,7 +13802,7 @@
     </row>
     <row r="4" spans="1:37" s="87" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52">
-        <v>0.366311288642309</v>
+        <v>0.17331083773112699</v>
       </c>
       <c r="B4" s="52">
         <v>0.19752813587260601</v>
@@ -13865,7 +13865,7 @@
     </row>
     <row r="5" spans="1:37" s="72" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53">
-        <v>0.53589812055320896</v>
+        <v>0.26011440433592897</v>
       </c>
       <c r="B5" s="53">
         <v>0.28527523866889698</v>
@@ -13928,7 +13928,7 @@
     </row>
     <row r="6" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <v>0.50572676643675296</v>
+        <v>0.34268029973736303</v>
       </c>
       <c r="B6" s="16">
         <v>0.33507944644200899</v>
@@ -13991,7 +13991,7 @@
     </row>
     <row r="7" spans="1:37" s="72" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="53">
-        <v>1.0607975763834501</v>
+        <v>0.64110879117637098</v>
       </c>
       <c r="B7" s="53">
         <v>0.58228513774475699</v>
@@ -14054,7 +14054,7 @@
     </row>
     <row r="8" spans="1:37" s="87" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
-        <v>1.3397914114497</v>
+        <v>0.85935328542174505</v>
       </c>
       <c r="B8" s="16">
         <v>0.79322921702375204</v>
@@ -14117,7 +14117,7 @@
     </row>
     <row r="9" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
-        <v>1.62393394477792</v>
+        <v>0.84804146882517595</v>
       </c>
       <c r="B9" s="16">
         <v>0.85499351566446002</v>
@@ -14180,7 +14180,7 @@
     </row>
     <row r="10" spans="1:37" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
-        <v>1.6927915275881</v>
+        <v>0.86721262376514197</v>
       </c>
       <c r="B10" s="16">
         <v>0.864483188317266</v>
@@ -14243,7 +14243,7 @@
     </row>
     <row r="11" spans="1:37" s="72" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="53">
-        <v>3.2537959810988299</v>
+        <v>2.6380634815189699</v>
       </c>
       <c r="B11" s="53">
         <v>1.7080133052945301</v>

</xml_diff>

<commit_message>
Finished up parameter tweaks for agreement contest figure 8. Added debugging code for contest code also. Recomputed r_delta_m for athero applied exmaples.
</commit_message>
<xml_diff>
--- a/mdm_z/atherosclerosis_review.xlsx
+++ b/mdm_z/atherosclerosis_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruce\Documents\CodeProjects\ACE\mdm_z\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDD87DF-3092-406A-A5BE-041BB20F4A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1518BF09-A042-4C78-B903-48437E9456CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
+    <workbookView xWindow="-19470" yWindow="840" windowWidth="18960" windowHeight="11835" activeTab="2" xr2:uid="{17CFB7B9-3BA9-45B4-964D-8FEC39BC2CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chol Null" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5143,7 +5142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5383,12 +5382,6 @@
     <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5407,13 +5400,34 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10180,7 +10194,7 @@
   <dimension ref="A1:AJ48"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10291,7 +10305,7 @@
     </row>
     <row r="3" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>0.119467592853033</v>
+        <v>0.121593125828345</v>
       </c>
       <c r="B3" s="30">
         <v>0.41129753907454902</v>
@@ -10309,7 +10323,7 @@
         <v>0.851980223093454</v>
       </c>
       <c r="G3" s="89">
-        <f t="shared" ref="G3:G12" si="0">-(I3-M3)/I3</f>
+        <f t="shared" ref="G3:G11" si="0">-(I3-M3)/I3</f>
         <v>-5.5072463768116052E-2</v>
       </c>
       <c r="H3" s="14" t="s">
@@ -10350,14 +10364,14 @@
       <c r="S3" s="17" t="s">
         <v>406</v>
       </c>
-      <c r="T3" s="102" t="s">
+      <c r="T3" s="100" t="s">
         <v>426</v>
       </c>
       <c r="Y3" s="48"/>
     </row>
     <row r="4" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
-        <v>0.16567496718522901</v>
+        <v>0.17184334993397399</v>
       </c>
       <c r="B4" s="28">
         <v>206.80477186439501</v>
@@ -10414,13 +10428,13 @@
       <c r="S4" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="T4" s="102" t="s">
+      <c r="T4" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
-        <v>0.17759148857781601</v>
+        <v>0.219693893758835</v>
       </c>
       <c r="B5" s="30">
         <v>0.467934886291557</v>
@@ -10483,7 +10497,7 @@
     </row>
     <row r="6" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <v>0.234556114439678</v>
+        <v>0.25081372019273901</v>
       </c>
       <c r="B6" s="30">
         <v>32.727260246574602</v>
@@ -10544,7 +10558,7 @@
     </row>
     <row r="7" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
-        <v>0.29060090781743703</v>
+        <v>0.30860369698662699</v>
       </c>
       <c r="B7" s="28">
         <v>729.20242348297995</v>
@@ -10601,13 +10615,13 @@
       <c r="S7" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="T7" s="102" t="s">
+      <c r="T7" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
-        <v>0.32864402272724402</v>
+        <v>0.30345351551815197</v>
       </c>
       <c r="B8" s="30">
         <v>33.980127101269801</v>
@@ -10666,13 +10680,13 @@
       <c r="S8" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="T8" s="102" t="s">
+      <c r="T8" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
-        <v>0.35372837090937498</v>
+        <v>0.44229019357833699</v>
       </c>
       <c r="B9" s="28">
         <v>476.91943102564102</v>
@@ -10730,13 +10744,13 @@
       <c r="S9" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="T9" s="102" t="s">
+      <c r="T9" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
-        <v>0.69484648624400602</v>
+        <v>0.79871378003520699</v>
       </c>
       <c r="B10" s="28">
         <v>391.43786617201903</v>
@@ -10799,7 +10813,7 @@
     </row>
     <row r="11" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
-        <v>1.13419239366617</v>
+        <v>1.5427763928473599</v>
       </c>
       <c r="B11" s="30">
         <v>10.473403683041999</v>
@@ -10856,19 +10870,19 @@
       <c r="S11" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="T11" s="102" t="s">
+      <c r="T11" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A12" s="105"/>
+      <c r="A12" s="101"/>
       <c r="B12" s="34"/>
       <c r="G12" s="16"/>
       <c r="H12" s="33"/>
       <c r="J12" s="28"/>
       <c r="L12" s="17"/>
       <c r="N12" s="30"/>
-      <c r="T12" s="102"/>
+      <c r="T12" s="100"/>
       <c r="U12" s="23"/>
       <c r="V12" s="23"/>
       <c r="W12" s="23"/>
@@ -10900,7 +10914,7 @@
       <c r="L13" s="17"/>
       <c r="N13" s="28"/>
       <c r="P13" s="29"/>
-      <c r="T13" s="102"/>
+      <c r="T13" s="100"/>
       <c r="U13" s="23"/>
       <c r="V13" s="23"/>
       <c r="W13" s="23"/>
@@ -12388,10 +12402,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:T8">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="569" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="568" priority="2">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13526,58 +13540,58 @@
     <sortCondition descending="1" ref="A3:A11"/>
   </sortState>
   <conditionalFormatting sqref="Q7:XFD7 N7:O7 Q13:XFD13 N2:XFD6 AB35:XFD35 A13:O13 A31:I31 K31:M31 A15:E15 A29 E29:L29 A18:M28 B1:XFD1 N8:XFD12 A14:XFD14 A32:XFD34 A36:XFD1048576 A35:O35 G15:XFD15 A2:M9 N17:XFD31 A30:M30 A16:XFD16">
-    <cfRule type="expression" dxfId="569" priority="37">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="568" priority="38">
+    <cfRule type="expression" dxfId="567" priority="37">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="566" priority="38">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29">
-    <cfRule type="expression" dxfId="567" priority="13">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="566" priority="14">
+    <cfRule type="expression" dxfId="565" priority="13">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="564" priority="14">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M29">
-    <cfRule type="expression" dxfId="565" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="564" priority="12">
+    <cfRule type="expression" dxfId="563" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="562" priority="12">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="expression" dxfId="563" priority="9">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="562" priority="10">
+    <cfRule type="expression" dxfId="561" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="560" priority="10">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10 E10:L10 A11:M12">
-    <cfRule type="expression" dxfId="561" priority="5">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="560" priority="6">
+    <cfRule type="expression" dxfId="559" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="558" priority="6">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:D10">
-    <cfRule type="expression" dxfId="559" priority="3">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="558" priority="4">
+    <cfRule type="expression" dxfId="557" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="556" priority="4">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="expression" dxfId="557" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="556" priority="2">
+    <cfRule type="expression" dxfId="555" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="554" priority="2">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13591,7 +13605,7 @@
   <dimension ref="A1:AJ44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:T11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="9" x14ac:dyDescent="0.15"/>
@@ -13717,12 +13731,12 @@
     </row>
     <row r="3" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
-        <v>0.13441159242109799</v>
+        <v>0.15587183086280601</v>
       </c>
       <c r="B3" s="40">
         <v>6.5599316794289297</v>
       </c>
-      <c r="C3" s="99">
+      <c r="C3" s="97">
         <v>0.61999379158845302</v>
       </c>
       <c r="D3" s="15">
@@ -13774,19 +13788,19 @@
       <c r="S3" s="91" t="s">
         <v>414</v>
       </c>
-      <c r="T3" s="102" t="s">
+      <c r="T3" s="100" t="s">
         <v>426</v>
       </c>
-      <c r="U3" s="102"/>
+      <c r="U3" s="100"/>
     </row>
     <row r="4" spans="1:36" s="85" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="50">
-        <v>0.17331083773112699</v>
+        <v>0.20303818219409001</v>
       </c>
       <c r="B4" s="44">
         <v>132047.55883083699</v>
       </c>
-      <c r="C4" s="100">
+      <c r="C4" s="98">
         <v>3.5713564070074102E-2</v>
       </c>
       <c r="D4" s="44">
@@ -13799,7 +13813,7 @@
         <v>0.42833084817045303</v>
       </c>
       <c r="G4" s="16">
-        <f t="shared" ref="G4:G11" si="0">(M4-I4)/I4</f>
+        <f>(M4-I4)/I4</f>
         <v>7.1802543006731492E-3</v>
       </c>
       <c r="H4" s="93" t="s">
@@ -13843,12 +13857,12 @@
     </row>
     <row r="5" spans="1:36" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="51">
-        <v>0.26011440433592897</v>
-      </c>
-      <c r="B5" s="97">
+        <v>0.26359851262496098</v>
+      </c>
+      <c r="B5" s="95">
         <v>104323.157854545</v>
       </c>
-      <c r="C5" s="101">
+      <c r="C5" s="99">
         <v>5.0486469068246699E-2</v>
       </c>
       <c r="D5" s="53">
@@ -13861,7 +13875,7 @@
         <v>0.35124519657054598</v>
       </c>
       <c r="G5" s="16">
-        <f t="shared" si="0"/>
+        <f>(M5-I5)/I5</f>
         <v>-1.9669504201611735E-2</v>
       </c>
       <c r="H5" s="52" t="s">
@@ -13900,18 +13914,18 @@
       <c r="S5" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="T5" s="102" t="s">
+      <c r="T5" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <v>0.34268029973736303</v>
+        <v>0.32910520157054102</v>
       </c>
       <c r="B6" s="28">
         <v>120.628600719123</v>
       </c>
-      <c r="C6" s="99">
+      <c r="C6" s="97">
         <v>0.91323124927187205</v>
       </c>
       <c r="D6" s="15">
@@ -13924,7 +13938,7 @@
         <v>1.2343254517573801</v>
       </c>
       <c r="G6" s="16">
-        <f t="shared" si="0"/>
+        <f>(M6-I6)/I6</f>
         <v>-0.18055555555555555</v>
       </c>
       <c r="H6" s="17" t="s">
@@ -13963,18 +13977,18 @@
       <c r="S6" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="T6" s="102" t="s">
+      <c r="T6" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:36" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="51">
-        <v>0.64110879117637098</v>
-      </c>
-      <c r="B7" s="98">
+        <v>0.50762085262478696</v>
+      </c>
+      <c r="B7" s="96">
         <v>13.450786681903899</v>
       </c>
-      <c r="C7" s="101">
+      <c r="C7" s="99">
         <v>0.39130715079531098</v>
       </c>
       <c r="D7" s="53">
@@ -13987,7 +14001,7 @@
         <v>0.53185997443182498</v>
       </c>
       <c r="G7" s="16">
-        <f t="shared" si="0"/>
+        <f>(M7-I7)/I7</f>
         <v>-0.16017316017316027</v>
       </c>
       <c r="H7" s="54" t="s">
@@ -14008,7 +14022,7 @@
       <c r="M7" s="53">
         <v>19.399999999999999</v>
       </c>
-      <c r="N7" s="98">
+      <c r="N7" s="96">
         <v>7.15</v>
       </c>
       <c r="O7" s="53">
@@ -14026,18 +14040,18 @@
       <c r="S7" s="52" t="s">
         <v>428</v>
       </c>
-      <c r="T7" s="102" t="s">
+      <c r="T7" s="100" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:36" s="85" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
-        <v>0.85935328542174505</v>
+        <v>1.0902953689300201</v>
       </c>
       <c r="B8" s="34">
         <v>0.56557243173793503</v>
       </c>
-      <c r="C8" s="99">
+      <c r="C8" s="97">
         <v>0.25180073430266697</v>
       </c>
       <c r="D8" s="15">
@@ -14050,7 +14064,7 @@
         <v>0.46608805098768102</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" si="0"/>
+        <f>(M8-I8)/I8</f>
         <v>-0.13464235624123419</v>
       </c>
       <c r="H8" s="93" t="s">
@@ -14089,144 +14103,144 @@
       <c r="S8" s="93" t="s">
         <v>301</v>
       </c>
-      <c r="T8" s="102" t="s">
+      <c r="T8" s="100" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
-        <v>0.84804146882517595</v>
-      </c>
-      <c r="B9" s="28">
+    <row r="9" spans="1:36" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="51">
+        <v>1.32890473186248</v>
+      </c>
+      <c r="B9" s="96">
+        <v>31.1213947794216</v>
+      </c>
+      <c r="C9" s="99">
+        <v>0.12847995194645101</v>
+      </c>
+      <c r="D9" s="53">
+        <v>0.744524617045352</v>
+      </c>
+      <c r="E9" s="53">
+        <v>0.63465869131768005</v>
+      </c>
+      <c r="F9" s="53">
+        <v>0.37030064190211498</v>
+      </c>
+      <c r="G9" s="51">
+        <f>(M9-I9)/I9</f>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="H9" s="104" t="s">
+        <v>424</v>
+      </c>
+      <c r="I9" s="105">
+        <v>36</v>
+      </c>
+      <c r="J9" s="105">
+        <v>23</v>
+      </c>
+      <c r="K9" s="105">
+        <v>15</v>
+      </c>
+      <c r="L9" s="104" t="s">
+        <v>425</v>
+      </c>
+      <c r="M9" s="105">
+        <v>41</v>
+      </c>
+      <c r="N9" s="105">
+        <v>50</v>
+      </c>
+      <c r="O9" s="105">
+        <v>13</v>
+      </c>
+      <c r="P9" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="105">
+        <v>0.05</v>
+      </c>
+      <c r="R9" s="105" t="s">
+        <v>312</v>
+      </c>
+      <c r="S9" s="104" t="s">
+        <v>313</v>
+      </c>
+      <c r="T9" s="106" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" s="85" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="50">
+        <v>2.2018381936729998</v>
+      </c>
+      <c r="B10" s="107">
         <v>260591.76365234001</v>
       </c>
-      <c r="C9" s="99">
+      <c r="C10" s="98">
         <v>3.9523876652813497E-2</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D10" s="44">
         <v>0.96246605138118502</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E10" s="44">
         <v>1</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F10" s="44">
         <v>0.54470925070932796</v>
       </c>
-      <c r="G9" s="16">
-        <f t="shared" si="0"/>
+      <c r="G10" s="50">
+        <f>(M10-I10)/I10</f>
         <v>1.8032205992361904E-2</v>
       </c>
-      <c r="H9" s="95" t="s">
+      <c r="H10" s="108" t="s">
         <v>291</v>
       </c>
-      <c r="I9" s="96">
+      <c r="I10" s="109">
         <v>304788</v>
       </c>
-      <c r="J9" s="96">
+      <c r="J10" s="109">
         <v>113425</v>
       </c>
-      <c r="K9" s="96">
+      <c r="K10" s="109">
         <v>4</v>
       </c>
-      <c r="L9" s="95" t="s">
+      <c r="L10" s="108" t="s">
         <v>341</v>
       </c>
-      <c r="M9" s="96">
+      <c r="M10" s="109">
         <v>310284</v>
       </c>
-      <c r="N9" s="96">
+      <c r="N10" s="109">
         <v>160647</v>
       </c>
-      <c r="O9" s="96">
+      <c r="O10" s="109">
         <v>3</v>
       </c>
-      <c r="P9" s="96" t="s">
+      <c r="P10" s="109" t="s">
         <v>419</v>
       </c>
-      <c r="Q9" s="96" t="s">
+      <c r="Q10" s="109" t="s">
         <v>359</v>
       </c>
-      <c r="R9" s="96" t="s">
+      <c r="R10" s="109" t="s">
         <v>332</v>
       </c>
-      <c r="S9" s="95" t="s">
+      <c r="S10" s="108" t="s">
         <v>339</v>
       </c>
-      <c r="T9" s="102" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
-        <v>0.86721262376514197</v>
-      </c>
-      <c r="B10" s="30">
-        <v>31.1213947794216</v>
-      </c>
-      <c r="C10" s="99">
-        <v>0.12847995194645101</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.744524617045352</v>
-      </c>
-      <c r="E10" s="15">
-        <v>0.63465869131768005</v>
-      </c>
-      <c r="F10" s="15">
-        <v>0.37030064190211498</v>
-      </c>
-      <c r="G10" s="16">
-        <f t="shared" si="0"/>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="H10" s="93" t="s">
-        <v>424</v>
-      </c>
-      <c r="I10" s="94">
-        <v>36</v>
-      </c>
-      <c r="J10" s="94">
-        <v>23</v>
-      </c>
-      <c r="K10" s="94">
-        <v>15</v>
-      </c>
-      <c r="L10" s="93" t="s">
-        <v>425</v>
-      </c>
-      <c r="M10" s="94">
-        <v>41</v>
-      </c>
-      <c r="N10" s="94">
-        <v>50</v>
-      </c>
-      <c r="O10" s="94">
-        <v>13</v>
-      </c>
-      <c r="P10" s="94" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" s="94">
-        <v>0.05</v>
-      </c>
-      <c r="R10" s="94" t="s">
-        <v>312</v>
-      </c>
-      <c r="S10" s="93" t="s">
-        <v>313</v>
-      </c>
-      <c r="T10" s="102" t="s">
+      <c r="T10" s="110" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:36" s="70" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51">
-        <v>2.6380634815189699</v>
-      </c>
-      <c r="B11" s="97">
+        <v>5.02369447699063</v>
+      </c>
+      <c r="B11" s="95">
         <v>17004.980467512301</v>
       </c>
-      <c r="C11" s="101">
+      <c r="C11" s="99">
         <v>0.57883864704215804</v>
       </c>
       <c r="D11" s="53">
@@ -14239,7 +14253,7 @@
         <v>1.0841311155647999</v>
       </c>
       <c r="G11" s="16">
-        <f t="shared" si="0"/>
+        <f>(M11-I11)/I11</f>
         <v>0.72719967858577739</v>
       </c>
       <c r="H11" s="52" t="s">
@@ -14248,7 +14262,7 @@
       <c r="I11" s="53">
         <v>9956</v>
       </c>
-      <c r="J11" s="97">
+      <c r="J11" s="95">
         <f>(12545-I11)*SQRT(K11)</f>
         <v>11578.359987493912</v>
       </c>
@@ -14261,7 +14275,7 @@
       <c r="M11" s="53">
         <v>17196</v>
       </c>
-      <c r="N11" s="97">
+      <c r="N11" s="95">
         <f>(20348-M11)*SQRT(O11)</f>
         <v>13372.803445799986</v>
       </c>
@@ -14280,7 +14294,7 @@
       <c r="S11" s="52" t="s">
         <v>405</v>
       </c>
-      <c r="T11" s="102" t="s">
+      <c r="T11" s="100" t="s">
         <v>426</v>
       </c>
     </row>
@@ -14308,11 +14322,7 @@
     <row r="14" spans="1:36" x14ac:dyDescent="0.15">
       <c r="B14" s="72"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
+    <row r="15" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="U15" s="73"/>
       <c r="V15" s="73"/>
       <c r="W15" s="73"/>
@@ -14535,15 +14545,15 @@
     </row>
     <row r="21" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="61">
-        <f t="shared" ref="A21:A38" si="1">B21/I21</f>
+        <f t="shared" ref="A21:A38" si="0">B21/I21</f>
         <v>0.30233492648200283</v>
       </c>
       <c r="B21" s="63">
-        <f t="shared" ref="B21:B38" si="2">ABS(M21-I21) + ABS(_xlfn.NORM.S.INV(1-(0.05/Q21)/2))*SQRT(J21^2/K21+N21^2/O21)</f>
+        <f t="shared" ref="B21:B38" si="1">ABS(M21-I21) + ABS(_xlfn.NORM.S.INV(1-(0.05/Q21)/2))*SQRT(J21^2/K21+N21^2/O21)</f>
         <v>110561.76626998305</v>
       </c>
       <c r="C21" s="61">
-        <f t="shared" ref="C21:C38" si="3">-(I21-M21)/I21</f>
+        <f t="shared" ref="C21:C38" si="2">-(I21-M21)/I21</f>
         <v>-1.9669504201611735E-2</v>
       </c>
       <c r="D21" s="76"/>
@@ -14605,15 +14615,15 @@
     </row>
     <row r="22" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="61">
+        <f t="shared" si="0"/>
+        <v>0.33187378676985985</v>
+      </c>
+      <c r="B22" s="67">
         <f t="shared" si="1"/>
-        <v>0.33187378676985985</v>
-      </c>
-      <c r="B22" s="67">
+        <v>8.5955310773393698</v>
+      </c>
+      <c r="C22" s="61">
         <f t="shared" si="2"/>
-        <v>8.5955310773393698</v>
-      </c>
-      <c r="C22" s="61">
-        <f t="shared" si="3"/>
         <v>-0.1274131274131273</v>
       </c>
       <c r="D22" s="76"/>
@@ -14677,15 +14687,15 @@
     </row>
     <row r="23" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="61">
+        <f t="shared" si="0"/>
+        <v>0.3351756133312177</v>
+      </c>
+      <c r="B23" s="63">
         <f t="shared" si="1"/>
-        <v>0.3351756133312177</v>
-      </c>
-      <c r="B23" s="63">
+        <v>8.7145659466116605</v>
+      </c>
+      <c r="C23" s="61">
         <f t="shared" si="2"/>
-        <v>8.7145659466116605</v>
-      </c>
-      <c r="C23" s="61">
-        <f t="shared" si="3"/>
         <v>4.2307692307692366E-2</v>
       </c>
       <c r="D23" s="76"/>
@@ -14749,15 +14759,15 @@
     </row>
     <row r="24" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="61">
+        <f t="shared" si="0"/>
+        <v>0.36468210626768915</v>
+      </c>
+      <c r="B24" s="68">
         <f t="shared" si="1"/>
-        <v>0.36468210626768915</v>
-      </c>
-      <c r="B24" s="68">
+        <v>131.28555825636809</v>
+      </c>
+      <c r="C24" s="61">
         <f t="shared" si="2"/>
-        <v>131.28555825636809</v>
-      </c>
-      <c r="C24" s="61">
-        <f t="shared" si="3"/>
         <v>-0.18055555555555555</v>
       </c>
       <c r="H24" s="58" t="s">
@@ -14799,15 +14809,15 @@
     </row>
     <row r="25" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="61">
+        <f t="shared" si="0"/>
+        <v>0.38375612642394952</v>
+      </c>
+      <c r="B25" s="63">
         <f t="shared" si="1"/>
-        <v>0.38375612642394952</v>
-      </c>
-      <c r="B25" s="63">
+        <v>127779.27741538247</v>
+      </c>
+      <c r="C25" s="61">
         <f t="shared" si="2"/>
-        <v>127779.27741538247</v>
-      </c>
-      <c r="C25" s="61">
-        <f t="shared" si="3"/>
         <v>4.5589692765113973E-2</v>
       </c>
       <c r="H25" s="58" t="s">
@@ -14851,15 +14861,15 @@
     </row>
     <row r="26" spans="1:36" s="59" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="61">
+        <f t="shared" si="0"/>
+        <v>0.43866397912473509</v>
+      </c>
+      <c r="B26" s="63">
         <f t="shared" si="1"/>
-        <v>0.43866397912473509</v>
-      </c>
-      <c r="B26" s="63">
+        <v>147.87362736294821</v>
+      </c>
+      <c r="C26" s="61">
         <f t="shared" si="2"/>
-        <v>147.87362736294821</v>
-      </c>
-      <c r="C26" s="61">
-        <f t="shared" si="3"/>
         <v>1.0382675763868287E-2</v>
       </c>
       <c r="H26" s="58" t="s">
@@ -14920,15 +14930,15 @@
     </row>
     <row r="27" spans="1:36" s="59" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="61">
+        <f t="shared" si="0"/>
+        <v>0.54447029123354107</v>
+      </c>
+      <c r="B27" s="63">
         <f t="shared" si="1"/>
-        <v>0.54447029123354107</v>
-      </c>
-      <c r="B27" s="63">
+        <v>65064.199802408162</v>
+      </c>
+      <c r="C27" s="61">
         <f t="shared" si="2"/>
-        <v>65064.199802408162</v>
-      </c>
-      <c r="C27" s="61">
-        <f t="shared" si="3"/>
         <v>-7.364016736401674E-2</v>
       </c>
       <c r="H27" s="58" t="s">
@@ -14989,15 +14999,15 @@
     </row>
     <row r="28" spans="1:36" s="59" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="61">
+        <f t="shared" si="0"/>
+        <v>0.59465772165882236</v>
+      </c>
+      <c r="B28" s="67">
         <f t="shared" si="1"/>
-        <v>0.59465772165882236</v>
-      </c>
-      <c r="B28" s="67">
+        <v>0.42399095554274036</v>
+      </c>
+      <c r="C28" s="61">
         <f t="shared" si="2"/>
-        <v>0.42399095554274036</v>
-      </c>
-      <c r="C28" s="61">
-        <f t="shared" si="3"/>
         <v>-1.542776998597477E-2</v>
       </c>
       <c r="H28" s="58" t="s">
@@ -15058,15 +15068,15 @@
     </row>
     <row r="29" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="61">
+        <f t="shared" si="0"/>
+        <v>0.62604580322464665</v>
+      </c>
+      <c r="B29" s="67">
         <f t="shared" si="1"/>
-        <v>0.62604580322464665</v>
-      </c>
-      <c r="B29" s="67">
+        <v>5.5718076486993548E-2</v>
+      </c>
+      <c r="C29" s="61">
         <f t="shared" si="2"/>
-        <v>5.5718076486993548E-2</v>
-      </c>
-      <c r="C29" s="61">
-        <f t="shared" si="3"/>
         <v>-0.3146067415730337</v>
       </c>
       <c r="H29" s="58" t="s">
@@ -15110,15 +15120,15 @@
     </row>
     <row r="30" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="61">
+        <f t="shared" si="0"/>
+        <v>0.64173877726018158</v>
+      </c>
+      <c r="B30" s="67">
         <f t="shared" si="1"/>
-        <v>0.64173877726018158</v>
-      </c>
-      <c r="B30" s="67">
+        <v>14.824165754710195</v>
+      </c>
+      <c r="C30" s="61">
         <f t="shared" si="2"/>
-        <v>14.824165754710195</v>
-      </c>
-      <c r="C30" s="61">
-        <f t="shared" si="3"/>
         <v>-0.16017316017316027</v>
       </c>
       <c r="H30" s="85" t="s">
@@ -15160,15 +15170,15 @@
     </row>
     <row r="31" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="61">
+        <f t="shared" si="0"/>
+        <v>0.72845716036649566</v>
+      </c>
+      <c r="B31" s="63">
         <f t="shared" si="1"/>
-        <v>0.72845716036649566</v>
-      </c>
-      <c r="B31" s="63">
+        <v>47087.470846090277</v>
+      </c>
+      <c r="C31" s="61">
         <f t="shared" si="2"/>
-        <v>47087.470846090277</v>
-      </c>
-      <c r="C31" s="61">
-        <f t="shared" si="3"/>
         <v>-0.16615099009900991</v>
       </c>
       <c r="H31" s="58" t="s">
@@ -15210,15 +15220,15 @@
     </row>
     <row r="32" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="61">
+        <f t="shared" si="0"/>
+        <v>0.87193649776221871</v>
+      </c>
+      <c r="B32" s="63">
         <f t="shared" si="1"/>
-        <v>0.87193649776221871</v>
-      </c>
-      <c r="B32" s="63">
+        <v>265755.7812799511</v>
+      </c>
+      <c r="C32" s="61">
         <f t="shared" si="2"/>
-        <v>265755.7812799511</v>
-      </c>
-      <c r="C32" s="61">
-        <f t="shared" si="3"/>
         <v>1.8032205992361904E-2</v>
       </c>
       <c r="H32" s="58" t="s">
@@ -15260,15 +15270,15 @@
     </row>
     <row r="33" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="61">
+        <f t="shared" si="0"/>
+        <v>0.90104148622149904</v>
+      </c>
+      <c r="B33" s="63">
         <f t="shared" si="1"/>
-        <v>0.90104148622149904</v>
-      </c>
-      <c r="B33" s="63">
+        <v>202294.53605041257</v>
+      </c>
+      <c r="C33" s="61">
         <f t="shared" si="2"/>
-        <v>202294.53605041257</v>
-      </c>
-      <c r="C33" s="61">
-        <f t="shared" si="3"/>
         <v>-0.22222385539474743</v>
       </c>
       <c r="H33" s="58" t="s">
@@ -15312,15 +15322,15 @@
     </row>
     <row r="34" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="61">
+        <f t="shared" si="0"/>
+        <v>0.93271875715240415</v>
+      </c>
+      <c r="B34" s="63">
         <f t="shared" si="1"/>
-        <v>0.93271875715240415</v>
-      </c>
-      <c r="B34" s="63">
+        <v>60253.631712045302</v>
+      </c>
+      <c r="C34" s="61">
         <f t="shared" si="2"/>
-        <v>60253.631712045302</v>
-      </c>
-      <c r="C34" s="61">
-        <f t="shared" si="3"/>
         <v>-0.16563467492260053</v>
       </c>
       <c r="H34" s="58" t="s">
@@ -15366,15 +15376,15 @@
     </row>
     <row r="35" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="61">
+        <f t="shared" si="0"/>
+        <v>0.96814672232900045</v>
+      </c>
+      <c r="B35" s="67">
         <f t="shared" si="1"/>
-        <v>0.96814672232900045</v>
-      </c>
-      <c r="B35" s="67">
+        <v>34.853282003844015</v>
+      </c>
+      <c r="C35" s="61">
         <f t="shared" si="2"/>
-        <v>34.853282003844015</v>
-      </c>
-      <c r="C35" s="61">
-        <f t="shared" si="3"/>
         <v>0.1388888888888889</v>
       </c>
       <c r="H35" s="58" t="s">
@@ -15418,15 +15428,15 @@
     </row>
     <row r="36" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="61">
+        <f t="shared" si="0"/>
+        <v>1.0072498831657288</v>
+      </c>
+      <c r="B36" s="63">
         <f t="shared" si="1"/>
-        <v>1.0072498831657288</v>
-      </c>
-      <c r="B36" s="63">
+        <v>391.71947956315188</v>
+      </c>
+      <c r="C36" s="61">
         <f t="shared" si="2"/>
-        <v>391.71947956315188</v>
-      </c>
-      <c r="C36" s="61">
-        <f t="shared" si="3"/>
         <v>-0.25739264592440209</v>
       </c>
       <c r="H36" s="58" t="s">
@@ -15468,15 +15478,15 @@
     </row>
     <row r="37" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="61">
+        <f t="shared" si="0"/>
+        <v>1.0221261204613394</v>
+      </c>
+      <c r="B37" s="63">
         <f t="shared" si="1"/>
-        <v>1.0221261204613394</v>
-      </c>
-      <c r="B37" s="63">
+        <v>38503.49095777866</v>
+      </c>
+      <c r="C37" s="61">
         <f t="shared" si="2"/>
-        <v>38503.49095777866</v>
-      </c>
-      <c r="C37" s="61">
-        <f t="shared" si="3"/>
         <v>-0.2808601008760287</v>
       </c>
       <c r="H37" s="58" t="s">
@@ -15518,15 +15528,15 @@
     </row>
     <row r="38" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="61">
+        <f t="shared" si="0"/>
+        <v>1.0559803904811791</v>
+      </c>
+      <c r="B38" s="63">
         <f t="shared" si="1"/>
-        <v>1.0559803904811791</v>
-      </c>
-      <c r="B38" s="63">
+        <v>68258.572440703414</v>
+      </c>
+      <c r="C38" s="61">
         <f t="shared" si="2"/>
-        <v>68258.572440703414</v>
-      </c>
-      <c r="C38" s="61">
-        <f t="shared" si="3"/>
         <v>-0.45730198019801982</v>
       </c>
       <c r="H38" s="58" t="s">
@@ -15872,1429 +15882,1429 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H23:O26 Q23:Q26 H27:Q27 H28:O28 I29:O29 I31:K31 M31:O31 H32:H33 H33:O33 I35:K35 M35:Q35 H36:O36 I37:K38 Q28 J32:Q32 H22:Q22 Q31 Q36 M37:Q38 Q33:Q34 U39:XFD39 K40:O40 H41:O41 Q40 H42:Q42 S36:S38 S21:S22 S28:S34 T41:XFD1048576 T21:XFD38 S40:XFD40 S19:XFD20 I43:K43 M43:R43 Q44 K44:O44 B12 T15:XFD15 U8:U11 X3:XFD6 X8:AB11 Y7:XFD7 U5:W6 V8:W10 V7 H40:I40 H19:Q20 B1:C1 H1:XFD1 H45:S1048576 H16:XFD18 H39:S39 S5 D3 H6:O7 Q6:Q7 H11:S11 D5:D7 G3:G12 H2:S2 U2:XFD2 V4:W4 H14:XFD14 H12:AB13 AH8:XFD13 A13:C14 A45:C1048576 A16:C19 A39:C40 A3:B3 A5:B11">
-    <cfRule type="expression" dxfId="555" priority="510">
+  <conditionalFormatting sqref="H23:O26 Q23:Q26 H27:Q27 H28:O28 I29:O29 I31:K31 M31:O31 H32:H33 H33:O33 I35:K35 M35:Q35 H36:O36 I37:K38 Q28 J32:Q32 H22:Q22 Q31 Q36 M37:Q38 Q33:Q34 U39:XFD39 K40:O40 H41:O41 Q40 H42:Q42 S36:S38 S21:S22 S28:S34 T41:XFD1048576 T21:XFD38 S40:XFD40 S19:XFD20 I43:K43 M43:R43 Q44 K44:O44 B12 U15:XFD15 U8:U11 X3:XFD6 X8:AB11 Y7:XFD7 U5:W6 V8:W10 V7 H40:I40 H19:Q20 B1:C1 H1:XFD1 H45:S1048576 H16:XFD18 H39:S39 S5 D3 H6:O7 Q6:Q7 H11:S11 D5:D7 H2:S2 U2:XFD2 V4:W4 H14:XFD14 H12:AB13 AH8:XFD13 A45:C1048576 A16:C19 A39:C40 A3:B3 G3:G8 D8:F8 G11:G12 A5:B11 D11:D12 D11:F11 A13:G14 D16:G1048576 D9:G10">
+    <cfRule type="expression" dxfId="553" priority="510">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P21 R5:R7 R11 A20:C22 A5:C6 A3:C3 A2:G2">
-    <cfRule type="expression" dxfId="554" priority="504">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="553" priority="505">
+    <cfRule type="expression" dxfId="552" priority="504">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="551" priority="505">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="552" priority="496">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="551" priority="497">
+    <cfRule type="expression" dxfId="550" priority="496">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="549" priority="497">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P23">
-    <cfRule type="expression" dxfId="550" priority="494">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="549" priority="495">
+    <cfRule type="expression" dxfId="548" priority="494">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="547" priority="495">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="548" priority="492">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="547" priority="493">
+    <cfRule type="expression" dxfId="546" priority="492">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="545" priority="493">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="546" priority="490">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="545" priority="491">
+    <cfRule type="expression" dxfId="544" priority="490">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="543" priority="491">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S24">
-    <cfRule type="expression" dxfId="544" priority="488">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="543" priority="489">
+    <cfRule type="expression" dxfId="542" priority="488">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="541" priority="489">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S25">
-    <cfRule type="expression" dxfId="542" priority="486">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="541" priority="487">
+    <cfRule type="expression" dxfId="540" priority="486">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="539" priority="487">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="540" priority="484">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="539" priority="485">
+    <cfRule type="expression" dxfId="538" priority="484">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="537" priority="485">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="538" priority="482">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="537" priority="483">
+    <cfRule type="expression" dxfId="536" priority="482">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="535" priority="483">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="expression" dxfId="536" priority="480">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="535" priority="481">
+    <cfRule type="expression" dxfId="534" priority="480">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="533" priority="481">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24">
-    <cfRule type="expression" dxfId="534" priority="478">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="533" priority="479">
+    <cfRule type="expression" dxfId="532" priority="478">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="531" priority="479">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="532" priority="476">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="531" priority="477">
+    <cfRule type="expression" dxfId="530" priority="476">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="529" priority="477">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="530" priority="474">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="529" priority="475">
+    <cfRule type="expression" dxfId="528" priority="474">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="527" priority="475">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="528" priority="472">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="527" priority="473">
+    <cfRule type="expression" dxfId="526" priority="472">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="525" priority="473">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P26">
-    <cfRule type="expression" dxfId="526" priority="470">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="525" priority="471">
+    <cfRule type="expression" dxfId="524" priority="470">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="523" priority="471">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="expression" dxfId="524" priority="468">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="523" priority="469">
+    <cfRule type="expression" dxfId="522" priority="468">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="521" priority="469">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="522" priority="466">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="521" priority="467">
+    <cfRule type="expression" dxfId="520" priority="466">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="519" priority="467">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="520" priority="464">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="519" priority="465">
+    <cfRule type="expression" dxfId="518" priority="464">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="517" priority="465">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="518" priority="462">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="517" priority="463">
+    <cfRule type="expression" dxfId="516" priority="462">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="515" priority="463">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S26">
-    <cfRule type="expression" dxfId="516" priority="460">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="515" priority="461">
+    <cfRule type="expression" dxfId="514" priority="460">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="513" priority="461">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S27">
-    <cfRule type="expression" dxfId="514" priority="458">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="513" priority="459">
+    <cfRule type="expression" dxfId="512" priority="458">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="511" priority="459">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="512" priority="456">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="511" priority="457">
+    <cfRule type="expression" dxfId="510" priority="456">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="509" priority="457">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="510" priority="454">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="509" priority="455">
+    <cfRule type="expression" dxfId="508" priority="454">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="507" priority="455">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="expression" dxfId="508" priority="452">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="507" priority="453">
+    <cfRule type="expression" dxfId="506" priority="452">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="505" priority="453">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28">
-    <cfRule type="expression" dxfId="506" priority="450">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="505" priority="451">
+    <cfRule type="expression" dxfId="504" priority="450">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="503" priority="451">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="expression" dxfId="504" priority="448">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="503" priority="449">
+    <cfRule type="expression" dxfId="502" priority="448">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="501" priority="449">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="502" priority="446">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="501" priority="447">
+    <cfRule type="expression" dxfId="500" priority="446">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="499" priority="447">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="expression" dxfId="500" priority="444">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="499" priority="445">
+    <cfRule type="expression" dxfId="498" priority="444">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="497" priority="445">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="498" priority="442">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="497" priority="443">
+    <cfRule type="expression" dxfId="496" priority="442">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="495" priority="443">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P29">
-    <cfRule type="expression" dxfId="496" priority="440">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="495" priority="441">
+    <cfRule type="expression" dxfId="494" priority="440">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="493" priority="441">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q29">
-    <cfRule type="expression" dxfId="494" priority="436">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="493" priority="437">
+    <cfRule type="expression" dxfId="492" priority="436">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="491" priority="437">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="expression" dxfId="492" priority="434">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="491" priority="435">
+    <cfRule type="expression" dxfId="490" priority="434">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="489" priority="435">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="490" priority="432">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="489" priority="433">
+    <cfRule type="expression" dxfId="488" priority="432">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="487" priority="433">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="488" priority="430">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="487" priority="431">
+    <cfRule type="expression" dxfId="486" priority="430">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="485" priority="431">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="486" priority="426">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="485" priority="427">
+    <cfRule type="expression" dxfId="484" priority="426">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="483" priority="427">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="484" priority="424">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="483" priority="425">
+    <cfRule type="expression" dxfId="482" priority="424">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="481" priority="425">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="482" priority="422">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="481" priority="423">
+    <cfRule type="expression" dxfId="480" priority="422">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="479" priority="423">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="expression" dxfId="480" priority="420">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="479" priority="421">
+    <cfRule type="expression" dxfId="478" priority="420">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="477" priority="421">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="expression" dxfId="478" priority="418">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="477" priority="419">
+    <cfRule type="expression" dxfId="476" priority="418">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="475" priority="419">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30">
-    <cfRule type="expression" dxfId="476" priority="416">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="475" priority="417">
+    <cfRule type="expression" dxfId="474" priority="416">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="473" priority="417">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30">
-    <cfRule type="expression" dxfId="474" priority="414">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="473" priority="415">
+    <cfRule type="expression" dxfId="472" priority="414">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="471" priority="415">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="expression" dxfId="472" priority="412">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="471" priority="413">
+    <cfRule type="expression" dxfId="470" priority="412">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="469" priority="413">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="470" priority="410">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="469" priority="411">
+    <cfRule type="expression" dxfId="468" priority="410">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="467" priority="411">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="468" priority="408">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="467" priority="409">
+    <cfRule type="expression" dxfId="466" priority="408">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="465" priority="409">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="466" priority="406">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="465" priority="407">
+    <cfRule type="expression" dxfId="464" priority="406">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="463" priority="407">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="464" priority="404">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="463" priority="405">
+    <cfRule type="expression" dxfId="462" priority="404">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="461" priority="405">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31">
-    <cfRule type="expression" dxfId="462" priority="402">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="461" priority="403">
+    <cfRule type="expression" dxfId="460" priority="402">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="459" priority="403">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31">
-    <cfRule type="expression" dxfId="460" priority="400">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="459" priority="401">
+    <cfRule type="expression" dxfId="458" priority="400">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="457" priority="401">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P31">
-    <cfRule type="expression" dxfId="458" priority="398">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="457" priority="399">
+    <cfRule type="expression" dxfId="456" priority="398">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="455" priority="399">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P31">
-    <cfRule type="expression" dxfId="456" priority="396">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="455" priority="397">
+    <cfRule type="expression" dxfId="454" priority="396">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="453" priority="397">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="454" priority="394">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="453" priority="395">
+    <cfRule type="expression" dxfId="452" priority="394">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="451" priority="395">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="452" priority="392">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="451" priority="393">
+    <cfRule type="expression" dxfId="450" priority="392">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="449" priority="393">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="expression" dxfId="450" priority="390">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="449" priority="391">
+    <cfRule type="expression" dxfId="448" priority="390">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="447" priority="391">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="448" priority="388">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="447" priority="389">
+    <cfRule type="expression" dxfId="446" priority="388">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="445" priority="389">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="expression" dxfId="446" priority="386">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="445" priority="387">
+    <cfRule type="expression" dxfId="444" priority="386">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="443" priority="387">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="444" priority="384">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="443" priority="385">
+    <cfRule type="expression" dxfId="442" priority="384">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="441" priority="385">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P33">
-    <cfRule type="expression" dxfId="442" priority="382">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="441" priority="383">
+    <cfRule type="expression" dxfId="440" priority="382">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="439" priority="383">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P33">
-    <cfRule type="expression" dxfId="440" priority="380">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="439" priority="381">
+    <cfRule type="expression" dxfId="438" priority="380">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="437" priority="381">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="expression" dxfId="438" priority="378">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="437" priority="379">
+    <cfRule type="expression" dxfId="436" priority="378">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="435" priority="379">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="436" priority="376">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="435" priority="377">
+    <cfRule type="expression" dxfId="434" priority="376">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="433" priority="377">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="expression" dxfId="434" priority="374">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="433" priority="375">
+    <cfRule type="expression" dxfId="432" priority="374">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="431" priority="375">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:K34 M34:O34">
-    <cfRule type="expression" dxfId="432" priority="364">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="431" priority="365">
+    <cfRule type="expression" dxfId="430" priority="364">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="429" priority="365">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="430" priority="362">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="429" priority="363">
+    <cfRule type="expression" dxfId="428" priority="362">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="427" priority="363">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="expression" dxfId="428" priority="360">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="427" priority="361">
+    <cfRule type="expression" dxfId="426" priority="360">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="425" priority="361">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34">
-    <cfRule type="expression" dxfId="426" priority="356">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="425" priority="357">
+    <cfRule type="expression" dxfId="424" priority="356">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="423" priority="357">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34">
-    <cfRule type="expression" dxfId="424" priority="358">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="423" priority="359">
+    <cfRule type="expression" dxfId="422" priority="358">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="421" priority="359">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34">
-    <cfRule type="expression" dxfId="422" priority="354">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="421" priority="355">
+    <cfRule type="expression" dxfId="420" priority="354">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="419" priority="355">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="420" priority="352">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="419" priority="353">
+    <cfRule type="expression" dxfId="418" priority="352">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="417" priority="353">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="418" priority="350">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="417" priority="351">
+    <cfRule type="expression" dxfId="416" priority="350">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="415" priority="351">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="416" priority="348">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="415" priority="349">
+    <cfRule type="expression" dxfId="414" priority="348">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="413" priority="349">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S35">
-    <cfRule type="expression" dxfId="414" priority="346">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="413" priority="347">
+    <cfRule type="expression" dxfId="412" priority="346">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="411" priority="347">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="412" priority="344">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="411" priority="345">
+    <cfRule type="expression" dxfId="410" priority="344">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="409" priority="345">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="410" priority="342">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="409" priority="343">
+    <cfRule type="expression" dxfId="408" priority="342">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="407" priority="343">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="expression" dxfId="408" priority="338">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="407" priority="339">
+    <cfRule type="expression" dxfId="406" priority="338">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="405" priority="339">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="expression" dxfId="406" priority="340">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="405" priority="341">
+    <cfRule type="expression" dxfId="404" priority="340">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="403" priority="341">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="404" priority="336">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="403" priority="337">
+    <cfRule type="expression" dxfId="402" priority="336">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="401" priority="337">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="402" priority="334">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="401" priority="335">
+    <cfRule type="expression" dxfId="400" priority="334">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="399" priority="335">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="400" priority="332">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="399" priority="333">
+    <cfRule type="expression" dxfId="398" priority="332">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="397" priority="333">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P36">
-    <cfRule type="expression" dxfId="398" priority="330">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="397" priority="331">
+    <cfRule type="expression" dxfId="396" priority="330">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="395" priority="331">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P36">
-    <cfRule type="expression" dxfId="396" priority="328">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="395" priority="329">
+    <cfRule type="expression" dxfId="394" priority="328">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="393" priority="329">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="394" priority="326">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="393" priority="327">
+    <cfRule type="expression" dxfId="392" priority="326">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="391" priority="327">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="392" priority="324">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="391" priority="325">
+    <cfRule type="expression" dxfId="390" priority="324">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="389" priority="325">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="390" priority="322">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="389" priority="323">
+    <cfRule type="expression" dxfId="388" priority="322">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="387" priority="323">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="388" priority="320">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="387" priority="321">
+    <cfRule type="expression" dxfId="386" priority="320">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="385" priority="321">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="expression" dxfId="386" priority="318">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="385" priority="319">
+    <cfRule type="expression" dxfId="384" priority="318">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="383" priority="319">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37">
-    <cfRule type="expression" dxfId="384" priority="316">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="383" priority="317">
+    <cfRule type="expression" dxfId="382" priority="316">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="381" priority="317">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37">
-    <cfRule type="expression" dxfId="382" priority="314">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="381" priority="315">
+    <cfRule type="expression" dxfId="380" priority="314">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="379" priority="315">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="380" priority="312">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="379" priority="313">
+    <cfRule type="expression" dxfId="378" priority="312">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="377" priority="313">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="expression" dxfId="378" priority="310">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="377" priority="311">
+    <cfRule type="expression" dxfId="376" priority="310">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="375" priority="311">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38">
-    <cfRule type="expression" dxfId="376" priority="308">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="375" priority="309">
+    <cfRule type="expression" dxfId="374" priority="308">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="373" priority="309">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38">
-    <cfRule type="expression" dxfId="374" priority="306">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="373" priority="307">
+    <cfRule type="expression" dxfId="372" priority="306">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="371" priority="307">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="372" priority="304">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="371" priority="305">
+    <cfRule type="expression" dxfId="370" priority="304">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="369" priority="305">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="370" priority="302">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="369" priority="303">
+    <cfRule type="expression" dxfId="368" priority="302">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="367" priority="303">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="expression" dxfId="368" priority="300">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="367" priority="301">
+    <cfRule type="expression" dxfId="366" priority="300">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="365" priority="301">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="366" priority="298">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="365" priority="299">
+    <cfRule type="expression" dxfId="364" priority="298">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="363" priority="299">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="364" priority="296">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="363" priority="297">
+    <cfRule type="expression" dxfId="362" priority="296">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="361" priority="297">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="362" priority="294">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="361" priority="295">
+    <cfRule type="expression" dxfId="360" priority="294">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="359" priority="295">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S41">
-    <cfRule type="expression" dxfId="360" priority="284">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="359" priority="285">
+    <cfRule type="expression" dxfId="358" priority="284">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="357" priority="285">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P40">
-    <cfRule type="expression" dxfId="358" priority="282">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="357" priority="283">
+    <cfRule type="expression" dxfId="356" priority="282">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="355" priority="283">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P41">
-    <cfRule type="expression" dxfId="356" priority="280">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="355" priority="281">
+    <cfRule type="expression" dxfId="354" priority="280">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="353" priority="281">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="354" priority="278">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="353" priority="279">
+    <cfRule type="expression" dxfId="352" priority="278">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="351" priority="279">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="352" priority="276">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="351" priority="277">
+    <cfRule type="expression" dxfId="350" priority="276">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="349" priority="277">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="expression" dxfId="350" priority="274">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="349" priority="275">
+    <cfRule type="expression" dxfId="348" priority="274">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="347" priority="275">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="348" priority="270">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="347" priority="271">
+    <cfRule type="expression" dxfId="346" priority="270">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="345" priority="271">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="346" priority="268">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="345" priority="269">
+    <cfRule type="expression" dxfId="344" priority="268">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="343" priority="269">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="344" priority="266">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="343" priority="267">
+    <cfRule type="expression" dxfId="342" priority="266">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="341" priority="267">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S42">
-    <cfRule type="expression" dxfId="342" priority="264">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="341" priority="265">
+    <cfRule type="expression" dxfId="340" priority="264">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="339" priority="265">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R42 R40 R19:R38">
-    <cfRule type="expression" dxfId="340" priority="262">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="339" priority="263">
+    <cfRule type="expression" dxfId="338" priority="262">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="337" priority="263">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S43">
-    <cfRule type="expression" dxfId="338" priority="260">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="337" priority="261">
+    <cfRule type="expression" dxfId="336" priority="260">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="335" priority="261">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="expression" dxfId="336" priority="258">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="335" priority="259">
+    <cfRule type="expression" dxfId="334" priority="258">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="333" priority="259">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="expression" dxfId="334" priority="248">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="333" priority="249">
+    <cfRule type="expression" dxfId="332" priority="248">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="331" priority="249">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43">
-    <cfRule type="expression" dxfId="332" priority="254">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="331" priority="255">
+    <cfRule type="expression" dxfId="330" priority="254">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="329" priority="255">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="330" priority="252">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="329" priority="253">
+    <cfRule type="expression" dxfId="328" priority="252">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="327" priority="253">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="328" priority="250">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="327" priority="251">
+    <cfRule type="expression" dxfId="326" priority="250">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="325" priority="251">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40">
-    <cfRule type="expression" dxfId="326" priority="246">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="325" priority="247">
+    <cfRule type="expression" dxfId="324" priority="246">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="323" priority="247">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R44:S44">
-    <cfRule type="expression" dxfId="324" priority="244">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="323" priority="245">
+    <cfRule type="expression" dxfId="322" priority="244">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="321" priority="245">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P44">
-    <cfRule type="expression" dxfId="322" priority="242">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="321" priority="243">
+    <cfRule type="expression" dxfId="320" priority="242">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="319" priority="243">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P44">
-    <cfRule type="expression" dxfId="320" priority="240">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="319" priority="241">
+    <cfRule type="expression" dxfId="318" priority="240">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="317" priority="241">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:I44">
-    <cfRule type="expression" dxfId="318" priority="238">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="317" priority="239">
+    <cfRule type="expression" dxfId="316" priority="238">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="315" priority="239">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="expression" dxfId="316" priority="232">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="315" priority="233">
+    <cfRule type="expression" dxfId="314" priority="232">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="313" priority="233">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="314" priority="236">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="313" priority="237">
+    <cfRule type="expression" dxfId="312" priority="236">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="311" priority="237">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="312" priority="234">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="311" priority="235">
+    <cfRule type="expression" dxfId="310" priority="234">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="309" priority="235">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="310" priority="230">
+    <cfRule type="expression" dxfId="308" priority="230">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="309" priority="227">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="308" priority="228">
+    <cfRule type="expression" dxfId="307" priority="227">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="306" priority="228">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="307" priority="137">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="306" priority="138">
+    <cfRule type="expression" dxfId="305" priority="137">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="304" priority="138">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:Q6 S6">
-    <cfRule type="expression" dxfId="305" priority="219">
+    <cfRule type="expression" dxfId="303" priority="219">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S7">
-    <cfRule type="expression" dxfId="304" priority="207">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="303" priority="208">
+    <cfRule type="expression" dxfId="302" priority="207">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="301" priority="208">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="302" priority="205">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="301" priority="206">
+    <cfRule type="expression" dxfId="300" priority="205">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="299" priority="206">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="expression" dxfId="300" priority="199">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="299" priority="200">
+    <cfRule type="expression" dxfId="298" priority="199">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="297" priority="200">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:K12 M12:R12">
-    <cfRule type="expression" dxfId="298" priority="196">
+    <cfRule type="expression" dxfId="296" priority="196">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12">
-    <cfRule type="expression" dxfId="297" priority="194">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="296" priority="195">
+    <cfRule type="expression" dxfId="295" priority="194">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="294" priority="195">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="295" priority="192">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="294" priority="193">
+    <cfRule type="expression" dxfId="293" priority="192">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="292" priority="193">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="293" priority="190">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="292" priority="191">
+    <cfRule type="expression" dxfId="291" priority="190">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="290" priority="191">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="291" priority="188">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="290" priority="189">
+    <cfRule type="expression" dxfId="289" priority="188">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="288" priority="189">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:O11 Q11 S11">
-    <cfRule type="expression" dxfId="289" priority="169">
-      <formula>MOD(ROW(),2)=0</formula>
+    <cfRule type="expression" dxfId="287" priority="169">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="286" priority="157">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="285" priority="158">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11">
+    <cfRule type="expression" dxfId="284" priority="151">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="283" priority="152">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P11">
+    <cfRule type="expression" dxfId="282" priority="149">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="281" priority="150">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="280" priority="147">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="279" priority="148">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" dxfId="278" priority="139">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="277" priority="140">
+      <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="288" priority="157">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="287" priority="158">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P11">
-    <cfRule type="expression" dxfId="286" priority="151">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="285" priority="152">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P11">
-    <cfRule type="expression" dxfId="284" priority="149">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="283" priority="150">
+    <cfRule type="expression" dxfId="276" priority="131">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="275" priority="132">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="274" priority="129">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="273" priority="130">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="272" priority="127">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="271" priority="128">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J44">
+    <cfRule type="expression" dxfId="270" priority="122">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="269" priority="96">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="268" priority="97">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:G1 E5:F7 E7:E8">
+    <cfRule type="expression" dxfId="267" priority="89">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="266" priority="86">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S6">
+    <cfRule type="expression" dxfId="265" priority="84">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="264" priority="85">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="263" priority="82">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="262" priority="83">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P6">
+    <cfRule type="expression" dxfId="261" priority="80">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="260" priority="81">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:K11 M11:R11">
+    <cfRule type="expression" dxfId="259" priority="79">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S11">
+    <cfRule type="expression" dxfId="258" priority="77">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="257" priority="78">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
+    <cfRule type="expression" dxfId="256" priority="75">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="255" priority="76">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11">
+    <cfRule type="expression" dxfId="254" priority="73">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="253" priority="74">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="282" priority="147">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="281" priority="148">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="280" priority="139">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="279" priority="140">
+    <cfRule type="expression" dxfId="252" priority="71">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="251" priority="72">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="250" priority="59">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="249" priority="60">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="278" priority="131">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="277" priority="132">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="276" priority="129">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="275" priority="130">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="274" priority="127">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="273" priority="128">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J44">
-    <cfRule type="expression" dxfId="272" priority="122">
-      <formula>MOD(ROW(),2)=0</formula>
+    <cfRule type="expression" dxfId="248" priority="53">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="247" priority="54">
+      <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="271" priority="96">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="270" priority="97">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D13:G1048576 D9:D12 D1:G1 E5:F7 D8:F11 E7:E8">
-    <cfRule type="expression" dxfId="269" priority="89">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="268" priority="86">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S6">
-    <cfRule type="expression" dxfId="267" priority="84">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="266" priority="85">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="265" priority="82">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="264" priority="83">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P6">
-    <cfRule type="expression" dxfId="263" priority="80">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="262" priority="81">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11:K11 M11:R11">
-    <cfRule type="expression" dxfId="261" priority="79">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="expression" dxfId="260" priority="77">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="259" priority="78">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="258" priority="75">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="257" priority="76">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L11">
-    <cfRule type="expression" dxfId="256" priority="73">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="255" priority="74">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="254" priority="71">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="253" priority="72">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="252" priority="59">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="251" priority="60">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="250" priority="53">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="249" priority="54">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="248" priority="48">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="247" priority="49">
+    <cfRule type="expression" dxfId="246" priority="48">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="245" priority="49">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="246" priority="46">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="245" priority="47">
+    <cfRule type="expression" dxfId="244" priority="46">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="243" priority="47">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="expression" dxfId="244" priority="44">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="243" priority="45">
+    <cfRule type="expression" dxfId="242" priority="44">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="241" priority="45">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="expression" dxfId="242" priority="29">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="241" priority="30">
+    <cfRule type="expression" dxfId="240" priority="29">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="239" priority="30">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="240" priority="27">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="239" priority="28">
+    <cfRule type="expression" dxfId="238" priority="27">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="237" priority="28">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="expression" dxfId="238" priority="25">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="237" priority="26">
+    <cfRule type="expression" dxfId="236" priority="25">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="235" priority="26">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S7">
-    <cfRule type="expression" dxfId="236" priority="41">
+    <cfRule type="expression" dxfId="234" priority="41">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="235" priority="39">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="234" priority="40">
+    <cfRule type="expression" dxfId="233" priority="39">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="232" priority="40">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="233" priority="37">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="232" priority="38">
+    <cfRule type="expression" dxfId="231" priority="37">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="230" priority="38">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="231" priority="35">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="230" priority="36">
+    <cfRule type="expression" dxfId="229" priority="35">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="228" priority="36">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="229" priority="33">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="228" priority="34">
+    <cfRule type="expression" dxfId="227" priority="33">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="226" priority="34">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="expression" dxfId="227" priority="31">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="226" priority="32">
+    <cfRule type="expression" dxfId="225" priority="31">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="224" priority="32">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2">
-    <cfRule type="expression" dxfId="225" priority="23">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="224" priority="24">
+    <cfRule type="expression" dxfId="223" priority="23">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="222" priority="24">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3">
-    <cfRule type="expression" dxfId="223" priority="21">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="222" priority="22">
+    <cfRule type="expression" dxfId="221" priority="21">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="220" priority="22">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U4">
-    <cfRule type="expression" dxfId="221" priority="19">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="220" priority="20">
+    <cfRule type="expression" dxfId="219" priority="19">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="218" priority="20">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5">
-    <cfRule type="expression" dxfId="219" priority="17">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="218" priority="18">
+    <cfRule type="expression" dxfId="217" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="216" priority="18">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3">
-    <cfRule type="expression" dxfId="217" priority="15">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="216" priority="16">
+    <cfRule type="expression" dxfId="215" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="214" priority="16">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6">
-    <cfRule type="expression" dxfId="215" priority="13">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="214" priority="14">
+    <cfRule type="expression" dxfId="213" priority="13">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="212" priority="14">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4">
-    <cfRule type="expression" dxfId="213" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="212" priority="12">
+    <cfRule type="expression" dxfId="211" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="210" priority="12">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T7">
-    <cfRule type="expression" dxfId="211" priority="9">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="210" priority="10">
+    <cfRule type="expression" dxfId="209" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="208" priority="10">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8">
-    <cfRule type="expression" dxfId="209" priority="7">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="208" priority="8">
+    <cfRule type="expression" dxfId="207" priority="7">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="206" priority="8">
+      <formula>"MOD(ROW(),2)=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T10">
+    <cfRule type="expression" dxfId="205" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="204" priority="6">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9">
-    <cfRule type="expression" dxfId="207" priority="5">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="206" priority="6">
-      <formula>"MOD(ROW(),2)=0"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T10">
-    <cfRule type="expression" dxfId="205" priority="3">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="204" priority="4">
+    <cfRule type="expression" dxfId="203" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="202" priority="4">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T11">
-    <cfRule type="expression" dxfId="203" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="202" priority="2">
+    <cfRule type="expression" dxfId="201" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="200" priority="2">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18653,806 +18663,806 @@
     <sortCondition descending="1" ref="A21:A37"/>
   </sortState>
   <conditionalFormatting sqref="P9:XFD9 P15:XFD15 AA35:XFD35 A31:I31 K31:M31 A20:M20 A17:E17 A2:M2 G27:K27 H26:K26 C26:E27 K29:M29 C29:E29 G29:I29 B33 K33:L33 E33:I33 A24:K24 L24:L28 G35:I35 C35:E35 K35:L35 A25:A31 B36:I36 N9 A15:N15 N2:XFD8 N10:XFD12 N19:XFD31 C22:E23 G22:L23 A21:A23 A1:XFD1 A13:XFD14 A16:XFD16 A38:XFD1048576 A18:XFD18 G17:XFD17 N33:XFD34 N35 K36:XFD36 N37:XFD37">
-    <cfRule type="expression" dxfId="201" priority="240">
+    <cfRule type="expression" dxfId="199" priority="240">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" dxfId="200" priority="230">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="199" priority="231">
+    <cfRule type="expression" dxfId="198" priority="230">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="197" priority="231">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21 D21:K21 M21">
-    <cfRule type="expression" dxfId="198" priority="228">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="197" priority="229">
+    <cfRule type="expression" dxfId="196" priority="228">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="195" priority="229">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M22">
-    <cfRule type="expression" dxfId="196" priority="226">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="195" priority="227">
+    <cfRule type="expression" dxfId="194" priority="226">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="193" priority="227">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="expression" dxfId="194" priority="224">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="193" priority="225">
+    <cfRule type="expression" dxfId="192" priority="224">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="191" priority="225">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="expression" dxfId="192" priority="222">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="191" priority="223">
+    <cfRule type="expression" dxfId="190" priority="222">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="189" priority="223">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M26">
-    <cfRule type="expression" dxfId="190" priority="218">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="189" priority="219">
+    <cfRule type="expression" dxfId="188" priority="218">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="187" priority="219">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M27">
-    <cfRule type="expression" dxfId="188" priority="216">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="187" priority="217">
+    <cfRule type="expression" dxfId="186" priority="216">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="185" priority="217">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="expression" dxfId="186" priority="204">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="185" priority="205">
+    <cfRule type="expression" dxfId="184" priority="204">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="183" priority="205">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="184" priority="212">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="183" priority="213">
+    <cfRule type="expression" dxfId="182" priority="212">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="181" priority="213">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="expression" dxfId="182" priority="210">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="181" priority="211">
+    <cfRule type="expression" dxfId="180" priority="210">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="179" priority="211">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31">
-    <cfRule type="expression" dxfId="180" priority="208">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="179" priority="209">
+    <cfRule type="expression" dxfId="178" priority="208">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="177" priority="209">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="178" priority="202">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="177" priority="203">
+    <cfRule type="expression" dxfId="176" priority="202">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="175" priority="203">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="expression" dxfId="176" priority="200">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="175" priority="201">
+    <cfRule type="expression" dxfId="174" priority="200">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="173" priority="201">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="expression" dxfId="174" priority="198">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="173" priority="199">
+    <cfRule type="expression" dxfId="172" priority="198">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="171" priority="199">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="172" priority="196">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="171" priority="197">
+    <cfRule type="expression" dxfId="170" priority="196">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="169" priority="197">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="expression" dxfId="170" priority="194">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="169" priority="195">
+    <cfRule type="expression" dxfId="168" priority="194">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="167" priority="195">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25">
-    <cfRule type="expression" dxfId="168" priority="192">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="167" priority="193">
+    <cfRule type="expression" dxfId="166" priority="192">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="165" priority="193">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="166" priority="190">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="165" priority="191">
+    <cfRule type="expression" dxfId="164" priority="190">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="191">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="164" priority="188">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="163" priority="189">
+    <cfRule type="expression" dxfId="162" priority="188">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="161" priority="189">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="expression" dxfId="162" priority="186">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="161" priority="187">
+    <cfRule type="expression" dxfId="160" priority="186">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="159" priority="187">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="expression" dxfId="160" priority="184">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="159" priority="185">
+    <cfRule type="expression" dxfId="158" priority="184">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="157" priority="185">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="expression" dxfId="158" priority="182">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="157" priority="183">
+    <cfRule type="expression" dxfId="156" priority="182">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="183">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25">
-    <cfRule type="expression" dxfId="156" priority="180">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="155" priority="181">
+    <cfRule type="expression" dxfId="154" priority="180">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="181">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="154" priority="168">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="153" priority="169">
+    <cfRule type="expression" dxfId="152" priority="168">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="151" priority="169">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E28 G28:K28 M28">
-    <cfRule type="expression" dxfId="152" priority="176">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="151" priority="177">
+    <cfRule type="expression" dxfId="150" priority="176">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="149" priority="177">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="150" priority="174">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="149" priority="175">
+    <cfRule type="expression" dxfId="148" priority="174">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="175">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="148" priority="172">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="147" priority="173">
+    <cfRule type="expression" dxfId="146" priority="172">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="173">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="expression" dxfId="146" priority="170">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="171">
+    <cfRule type="expression" dxfId="144" priority="170">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="171">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29">
-    <cfRule type="expression" dxfId="144" priority="166">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="143" priority="167">
+    <cfRule type="expression" dxfId="142" priority="166">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="167">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="142" priority="164">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="141" priority="165">
+    <cfRule type="expression" dxfId="140" priority="164">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="165">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="140" priority="162">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="139" priority="163">
+    <cfRule type="expression" dxfId="138" priority="162">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="163">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="expression" dxfId="138" priority="158">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="137" priority="159">
+    <cfRule type="expression" dxfId="136" priority="158">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="135" priority="159">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="expression" dxfId="136" priority="160">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="161">
+    <cfRule type="expression" dxfId="134" priority="160">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="161">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:M30">
-    <cfRule type="expression" dxfId="134" priority="156">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="133" priority="157">
+    <cfRule type="expression" dxfId="132" priority="156">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="131" priority="157">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P32:XFD32">
-    <cfRule type="expression" dxfId="132" priority="154">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="131" priority="155">
+    <cfRule type="expression" dxfId="130" priority="154">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="155">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="expression" dxfId="130" priority="152">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="129" priority="153">
+    <cfRule type="expression" dxfId="128" priority="152">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="153">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="128" priority="144">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="145">
+    <cfRule type="expression" dxfId="126" priority="144">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="145">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M33">
-    <cfRule type="expression" dxfId="126" priority="142">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="125" priority="143">
+    <cfRule type="expression" dxfId="124" priority="142">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="123" priority="143">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33">
-    <cfRule type="expression" dxfId="124" priority="140">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="123" priority="141">
+    <cfRule type="expression" dxfId="122" priority="140">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="141">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:D33">
-    <cfRule type="expression" dxfId="122" priority="138">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="121" priority="139">
+    <cfRule type="expression" dxfId="120" priority="138">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="119" priority="139">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:A34">
-    <cfRule type="expression" dxfId="120" priority="136">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="119" priority="137">
+    <cfRule type="expression" dxfId="118" priority="136">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="137">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34">
-    <cfRule type="expression" dxfId="118" priority="128">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="129">
+    <cfRule type="expression" dxfId="116" priority="128">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="129">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:K34">
-    <cfRule type="expression" dxfId="116" priority="132">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="133">
+    <cfRule type="expression" dxfId="114" priority="132">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="133">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M34">
-    <cfRule type="expression" dxfId="114" priority="130">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="131">
+    <cfRule type="expression" dxfId="112" priority="130">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="131">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="expression" dxfId="112" priority="126">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="127">
+    <cfRule type="expression" dxfId="110" priority="126">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="127">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35">
-    <cfRule type="expression" dxfId="110" priority="124">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="125">
+    <cfRule type="expression" dxfId="108" priority="124">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="107" priority="125">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="expression" dxfId="108" priority="122">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="123">
+    <cfRule type="expression" dxfId="106" priority="122">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="123">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="106" priority="120">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="121">
+    <cfRule type="expression" dxfId="104" priority="120">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="121">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="expression" dxfId="104" priority="118">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="119">
+    <cfRule type="expression" dxfId="102" priority="118">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="119">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:A36">
-    <cfRule type="expression" dxfId="102" priority="116">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="117">
+    <cfRule type="expression" dxfId="100" priority="116">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="117">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22">
-    <cfRule type="expression" dxfId="100" priority="114">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="99" priority="115">
+    <cfRule type="expression" dxfId="98" priority="114">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="115">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="98" priority="112">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="97" priority="113">
+    <cfRule type="expression" dxfId="96" priority="112">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="113">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="96" priority="110">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="111">
+    <cfRule type="expression" dxfId="94" priority="110">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="111">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36">
-    <cfRule type="expression" dxfId="94" priority="104">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="105">
+    <cfRule type="expression" dxfId="92" priority="104">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="105">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36">
-    <cfRule type="expression" dxfId="92" priority="106">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="107">
+    <cfRule type="expression" dxfId="90" priority="106">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="107">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="90" priority="102">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="103">
+    <cfRule type="expression" dxfId="88" priority="102">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="103">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="expression" dxfId="88" priority="100">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="101">
+    <cfRule type="expression" dxfId="86" priority="100">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="101">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="expression" dxfId="86" priority="98">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="99">
+    <cfRule type="expression" dxfId="84" priority="98">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="99">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="expression" dxfId="84" priority="96">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="97">
+    <cfRule type="expression" dxfId="82" priority="96">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="97">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:M37">
-    <cfRule type="expression" dxfId="82" priority="94">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="95">
+    <cfRule type="expression" dxfId="80" priority="94">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="95">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:E4 G4:J4 A3:A4 L4">
-    <cfRule type="expression" dxfId="80" priority="92">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="93">
+    <cfRule type="expression" dxfId="78" priority="92">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="77" priority="93">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 D3:K3 M3">
-    <cfRule type="expression" dxfId="78" priority="90">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="91">
+    <cfRule type="expression" dxfId="76" priority="90">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="91">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4">
-    <cfRule type="expression" dxfId="76" priority="88">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="89">
+    <cfRule type="expression" dxfId="74" priority="88">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="89">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="74" priority="86">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="87">
+    <cfRule type="expression" dxfId="72" priority="86">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="87">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="expression" dxfId="72" priority="84">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="71" priority="85">
+    <cfRule type="expression" dxfId="70" priority="84">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="85">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="expression" dxfId="70" priority="82">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="83">
+    <cfRule type="expression" dxfId="68" priority="82">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="83">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="68" priority="80">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="81">
+    <cfRule type="expression" dxfId="66" priority="80">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="65" priority="81">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:M8 C8:E8 G8:I8 L7 A7:A8">
-    <cfRule type="expression" dxfId="66" priority="78">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="79">
+    <cfRule type="expression" dxfId="64" priority="78">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="79">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="64" priority="68">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="69">
+    <cfRule type="expression" dxfId="62" priority="68">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="69">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7 G7:K7 M7">
-    <cfRule type="expression" dxfId="62" priority="76">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="77">
+    <cfRule type="expression" dxfId="60" priority="76">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="77">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="60" priority="74">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="75">
+    <cfRule type="expression" dxfId="58" priority="74">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="75">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="58" priority="72">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="73">
+    <cfRule type="expression" dxfId="56" priority="72">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="73">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="56" priority="70">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="71">
+    <cfRule type="expression" dxfId="54" priority="70">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="53" priority="71">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="54" priority="66">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="67">
+    <cfRule type="expression" dxfId="52" priority="66">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="51" priority="67">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="52" priority="64">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="65">
+    <cfRule type="expression" dxfId="50" priority="64">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="65">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="50" priority="62">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63">
+    <cfRule type="expression" dxfId="48" priority="62">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="63">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="48" priority="58">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="59">
+    <cfRule type="expression" dxfId="46" priority="58">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="59">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="46" priority="60">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="61">
+    <cfRule type="expression" dxfId="44" priority="60">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="61">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:M11">
-    <cfRule type="expression" dxfId="44" priority="56">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="57">
+    <cfRule type="expression" dxfId="42" priority="56">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="57">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="42" priority="42">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="43">
+    <cfRule type="expression" dxfId="40" priority="42">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="43">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="40" priority="40">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="41">
+    <cfRule type="expression" dxfId="38" priority="40">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="41">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10 L10 E10:I10">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="36" priority="39">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="expression" dxfId="37" priority="37">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="38">
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="expression" dxfId="35" priority="35">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="36">
+    <cfRule type="expression" dxfId="33" priority="35">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="36">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:D10">
-    <cfRule type="expression" dxfId="33" priority="33">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="34">
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="34">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="31" priority="31">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32">
+    <cfRule type="expression" dxfId="29" priority="31">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:E5 G5:J5 A5 L5">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="27" priority="30">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="28" priority="28">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="26" priority="28">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="26" priority="26">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="27">
+    <cfRule type="expression" dxfId="24" priority="26">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="27">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="24" priority="24">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="22" priority="24">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="25">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="22" priority="22">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="23">
+    <cfRule type="expression" dxfId="20" priority="22">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="23">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
+    <cfRule type="expression" dxfId="18" priority="20">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:J6 L6">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="16" priority="19">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="expression" dxfId="17" priority="17">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="15" priority="17">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="18">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="15" priority="15">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="13" priority="15">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="13" priority="13">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="12">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>"MOD(ROW(),2)=0"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19485,31 +19495,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="H2" s="103" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="H2" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103" t="s">
+      <c r="I2" s="102"/>
+      <c r="J2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="103"/>
+      <c r="K2" s="102"/>
       <c r="L2" s="2"/>
-      <c r="N2" s="103" t="s">
+      <c r="N2" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
     </row>
     <row r="3" spans="2:21" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">

</xml_diff>